<commit_message>
changed dqs to delta_qs
</commit_message>
<xml_diff>
--- a/Data/Hardy_Cross_network_flow_output.xlsx
+++ b/Data/Hardy_Cross_network_flow_output.xlsx
@@ -135,12 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,117 +464,117 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>124</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>13.4562984766708</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>160</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>0.00414001241052633</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>0.513361538905265</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>0.0381000129620584</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>90</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>10.1151497029193</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>140</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>0.00473388923396997</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>0.426050031057297</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>0.0420461974466528</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>126</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>2.00358692965692</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>75</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>0.00530061708094545</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <v>0.667877752199127</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>0.334328224522886</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>92</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>-5.39205290531708</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>90</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>0.0127582781480481</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <v>-1.17376158962043</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>0.217853650569492</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>110</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>-12.6896992967328</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>160</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>0.00372663121271842</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6">
         <v>-0.409929433399026</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>0.0322974632129799</v>
       </c>
     </row>
@@ -616,94 +615,94 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>126</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>-2.01995104354626</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>75</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>0.00541164875920303</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>-0.681867743659582</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>0.337334511211318</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>110</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>3.00541127506002</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>75</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>0.0109816030854207</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>1.20797633939628</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>0.399757157270476</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>100</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>2.01294936710504</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>63</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>0.0124959532544132</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <v>1.24959532544132</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>0.615772445777576</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>108</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>-2.32221656455035</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>63</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>0.0158086615144545</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <v>-1.70733544356109</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>0.736111741055709</v>
       </c>
     </row>
@@ -744,117 +743,117 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>92</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>5.3745202034551</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>90</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>0.0127018828946048</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>1.16857322630364</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>0.217437296758729</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>108</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>2.30468386268837</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>63</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>0.0156465419520165</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>1.68982653081778</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>0.732842437656131</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>100</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>-3.46432360453352</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>75</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>0.0138437770746075</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <v>-1.38437770746075</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>0.401642497776047</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>200</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>-8.14817702568045</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>125</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>0.00551092110207525</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <v>-1.10218422041505</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>0.135559271383479</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>136</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>-2.03803757211878</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>90</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>0.0023108740813206</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6">
         <v>-0.314278875059602</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>0.153992658227205</v>
       </c>
     </row>
@@ -895,94 +894,94 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>160</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>-17.1141882476644</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>160</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>0.00629837732087839</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>-1.00774037134054</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>0.0589267333623729</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>104</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>7.59574068967514</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>140</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>0.00285888968344498</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>0.297324527078278</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>0.0390787296282534</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>136</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>2.02543147297415</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>90</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>0.00227044508433721</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <v>0.30878053146986</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>0.152823453194951</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>110</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>12.6770931975881</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>160</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>0.00371611416437082</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <v>0.40877255808079</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>0.0322580723625685</v>
       </c>
     </row>

</xml_diff>